<commit_message>
added information for ER
</commit_message>
<xml_diff>
--- a/templates/2EXT03_Metabolites/2EXT03_Metabolites.xlsx
+++ b/templates/2EXT03_Metabolites/2EXT03_Metabolites.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT03_Metabolites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\SWATE_templates\templates\2EXT03_Metabolites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384BF54A-0A77-4FAB-A8E6-AD15F5363CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3EEEC-69C2-400E-A875-408EC6ED9ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{682F0441-A0F7-6741-B76C-DF63FF53992B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Source Name</t>
   </si>
@@ -284,6 +284,36 @@
   </si>
   <si>
     <t>The name of the input (the source) of this assay.</t>
+  </si>
+  <si>
+    <t>Term Source REF [MS derivatization] (#h; #tNFDI4PSO:0000052)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [MS derivatization] (#h; #tNFDI4PSO:0000052)</t>
+  </si>
+  <si>
+    <t>A unique identifier from a particular source (a batch of samples can have a unique Sample name as identified in the Sample table). It’s usually associated with an output spectral data filename.</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>EXTRACTION - Post Extraction</t>
+  </si>
+  <si>
+    <t>This how the sample was extracted into a solvent prior to being injected into the analytical instrument of choice.</t>
+  </si>
+  <si>
+    <t>EXTRACTION - Extract Name</t>
+  </si>
+  <si>
+    <t>Leave blank if you don’t have one.</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -294,7 +324,7 @@
     <numFmt numFmtId="164" formatCode="0.00\ &quot;microliter&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;microgram&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -356,6 +386,17 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -451,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,6 +610,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -603,9 +650,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D2F4E0D-C0CD-5F4A-8873-824BF4046AF1}" name="annotationTable" displayName="annotationTable" ref="D2:W3" totalsRowShown="0">
-  <autoFilter ref="D2:W3" xr:uid="{B8CBCCDE-BB9A-1943-AF13-CF08D39F25EB}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D2F4E0D-C0CD-5F4A-8873-824BF4046AF1}" name="annotationTable" displayName="annotationTable" ref="D2:Y3" totalsRowShown="0">
+  <autoFilter ref="D2:Y3" xr:uid="{B8CBCCDE-BB9A-1943-AF13-CF08D39F25EB}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{3998B63E-8A32-8B43-A9F8-6B28BA709419}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{B0972144-49CE-1D49-B224-1CC170522482}" name="Sample Name"/>
     <tableColumn id="3" xr3:uid="{77AF736E-56D5-7F44-A162-A7D79B145D0A}" name="Parameter [Bio entity]" dataDxfId="3"/>
@@ -626,6 +673,8 @@
     <tableColumn id="15" xr3:uid="{62EB9B8C-50C0-6846-8385-0ECF0EEA3C7A}" name="Unit [microliter] (#h; #tUO:0000101; #u)"/>
     <tableColumn id="16" xr3:uid="{72DC9DFD-4689-034A-BBD8-638D9FD59658}" name="Term Source REF [microliter] (#h; #tUO:0000101; #u)"/>
     <tableColumn id="17" xr3:uid="{DA5CEEFD-FC2F-5F4E-92BF-2EDE31FDC7EF}" name="Term Accession Number [microliter] (#h; #tUO:0000101; #u)"/>
+    <tableColumn id="22" xr3:uid="{BEB1A7F9-A26B-4E29-B74D-C938D021193B}" name="Term Source REF [MS derivatization] (#h; #tNFDI4PSO:0000052)"/>
+    <tableColumn id="23" xr3:uid="{8028DB47-142F-4FD8-BC4F-2CD8CA277263}" name="Term Accession Number [MS derivatization] (#h; #tNFDI4PSO:0000052)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -928,7 +977,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="549" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -946,13 +995,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CE882A-09A3-2E4E-BDAD-167459C0EEF7}">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -960,30 +1009,32 @@
     <col min="1" max="1" width="22.5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.125" style="22" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="61.375" style="22" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="32.625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.375" style="22" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="68.625" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="41.5" style="22" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="53.375" style="22" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="59.875" style="22" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="41.375" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="61.875" style="22" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="68.125" style="22" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="39.5" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="69.125" style="22" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="75.625" style="22" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="40.5" style="22" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="52.375" style="22" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="58.5" style="22" hidden="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.875" style="22"/>
+    <col min="4" max="4" width="42.75" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.125" style="22" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="58.875" style="22" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="30.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.625" style="22" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="66.375" style="22" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="39.375" style="22" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="50.25" style="22" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="57" style="22" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="50.875" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="58.375" style="22" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="65.25" style="22" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="39.625" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="65.625" style="22" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="72.375" style="22" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="38.625" style="22" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="49.5" style="22" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="56.25" style="22" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="58.875" style="22" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="65.75" style="22" hidden="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -1010,9 +1061,11 @@
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>49</v>
       </c>
@@ -1078,8 +1131,14 @@
       <c r="W2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>49</v>
       </c>
@@ -1105,8 +1164,10 @@
       <c r="U3"/>
       <c r="V3"/>
       <c r="W3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3"/>
+      <c r="Y3"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1131,7 +1192,7 @@
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>51</v>
       </c>
@@ -1164,7 +1225,7 @@
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>51</v>
       </c>
@@ -1197,7 +1258,7 @@
       <c r="V6" s="15"/>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>51</v>
       </c>
@@ -1228,7 +1289,7 @@
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>51</v>
       </c>
@@ -1259,7 +1320,7 @@
       <c r="V8" s="15"/>
       <c r="W8" s="15"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>51</v>
       </c>
@@ -1288,7 +1349,7 @@
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>51</v>
       </c>
@@ -1309,13 +1370,8 @@
       <c r="P10" s="15"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1334,13 +1390,13 @@
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-    </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>52</v>
       </c>
@@ -1373,13 +1429,13 @@
       <c r="R12" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="17"/>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>52</v>
       </c>
@@ -1412,13 +1468,13 @@
       <c r="R13" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>52</v>
       </c>
@@ -1449,7 +1505,7 @@
       <c r="V14" s="18"/>
       <c r="W14" s="18"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>52</v>
       </c>
@@ -1484,7 +1540,7 @@
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1782,7 @@
       <c r="V23" s="21"/>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" s="29" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="37" t="s">
         <v>27</v>
       </c>
@@ -1736,8 +1792,12 @@
       <c r="C24" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="D24" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>89</v>
+      </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -1747,7 +1807,9 @@
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
+      <c r="O24" s="48" t="s">
+        <v>87</v>
+      </c>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
@@ -1757,7 +1819,7 @@
       <c r="V24" s="15"/>
       <c r="W24" s="15"/>
     </row>
-    <row r="25" spans="1:23" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" s="29" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
         <v>27</v>
       </c>
@@ -1767,8 +1829,12 @@
       <c r="C25" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>90</v>
+      </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -1778,7 +1844,9 @@
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
+      <c r="O25" s="48" t="s">
+        <v>88</v>
+      </c>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
@@ -1788,7 +1856,7 @@
       <c r="V25" s="15"/>
       <c r="W25" s="15"/>
     </row>
-    <row r="26" spans="1:23" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>27</v>
       </c>
@@ -1798,8 +1866,12 @@
       <c r="C26" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="D26" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>91</v>
+      </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -1809,7 +1881,9 @@
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
+      <c r="O26" s="48" t="s">
+        <v>85</v>
+      </c>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
@@ -1819,7 +1893,7 @@
       <c r="V26" s="15"/>
       <c r="W26" s="15"/>
     </row>
-    <row r="27" spans="1:23" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" s="29" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
         <v>27</v>
       </c>
@@ -1829,8 +1903,12 @@
       <c r="C27" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>86</v>
+      </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -1840,7 +1918,9 @@
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
+      <c r="O27" s="48" t="s">
+        <v>86</v>
+      </c>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
@@ -1938,6 +2018,7 @@
       <c r="W30" s="14"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
[test] added Protocol REF column to template
</commit_message>
<xml_diff>
--- a/templates/2EXT03_Metabolites/2EXT03_Metabolites.xlsx
+++ b/templates/2EXT03_Metabolites/2EXT03_Metabolites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\2EXT03_Metabolites\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/2EXT03_Metabolites/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A306E02B-A8E5-4F79-B434-92283C61B383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2C143F-8BF2-6049-8AC3-FFA7CC92F5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{682F0441-A0F7-6741-B76C-DF63FF53992B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{682F0441-A0F7-6741-B76C-DF63FF53992B}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT03_Metabolites" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Source Name</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>This is how the sample was extracted into a solvent prior to being injected into the analytical instrument of choice.</t>
+  </si>
+  <si>
+    <t>Protocol REF</t>
+  </si>
+  <si>
+    <t>Extraction</t>
   </si>
 </sst>
 </file>
@@ -447,9 +453,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{B40B955E-1452-134F-8253-D50D28A6309D}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -478,11 +484,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D2F4E0D-C0CD-5F4A-8873-824BF4046AF1}" name="annotationTable" displayName="annotationTable" ref="C2:V21" totalsRowShown="0">
-  <autoFilter ref="C2:V21" xr:uid="{B8CBCCDE-BB9A-1943-AF13-CF08D39F25EB}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D2F4E0D-C0CD-5F4A-8873-824BF4046AF1}" name="annotationTable" displayName="annotationTable" ref="C2:W21" totalsRowShown="0">
+  <autoFilter ref="C2:W21" xr:uid="{B8CBCCDE-BB9A-1943-AF13-CF08D39F25EB}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{3998B63E-8A32-8B43-A9F8-6B28BA709419}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{B0972144-49CE-1D49-B224-1CC170522482}" name="Sample Name"/>
+    <tableColumn id="21" xr3:uid="{B36C1C65-C25E-884C-A546-1BFA119D318F}" name="Protocol REF"/>
     <tableColumn id="3" xr3:uid="{77AF736E-56D5-7F44-A162-A7D79B145D0A}" name="Parameter [Bio entity]" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5AFF8057-B228-184D-957B-38ADC417EEC9}" name="Term Source REF [Bio entity] (#h; #tNFDI4PSO:0000012)"/>
     <tableColumn id="5" xr3:uid="{A24CE6BE-0369-E64C-BAC0-E00C061D43E7}" name="Term Accession Number [Bio entity] (#h; #tNFDI4PSO:0000012)"/>
@@ -507,7 +514,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -821,43 +828,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CE882A-09A3-2E4E-BDAD-167459C0EEF7}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="14" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.5" style="14" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="59.875" style="14" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61" style="14" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="67.375" style="14" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="40.375" style="14" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="51.875" style="14" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="58.375" style="14" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="50.375" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="60" style="14" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="66.125" style="14" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="37" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.875" style="14" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="73.125" style="14" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="39.125" style="14" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="50.625" style="14" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="56.875" style="14" hidden="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.875" style="14"/>
+    <col min="2" max="2" width="34.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.5" style="14" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="59.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="61" style="14" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="67.33203125" style="14" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="40.33203125" style="14" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="51.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="58.33203125" style="14" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="50.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="60" style="14" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="66.1640625" style="14" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="37" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="66.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="73.1640625" style="14" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="39.1640625" style="14" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="50.6640625" style="14" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="56.83203125" style="14" hidden="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
@@ -884,8 +892,9 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>35</v>
       </c>
@@ -897,308 +906,322 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>8</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>9</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>12</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>14</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>15</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3"/>
       <c r="D3"/>
-      <c r="E3" s="2"/>
-      <c r="F3"/>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2"/>
       <c r="G3"/>
-      <c r="H3" s="5"/>
-      <c r="I3"/>
+      <c r="H3"/>
+      <c r="I3" s="5"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
-      <c r="N3" s="2"/>
-      <c r="O3"/>
+      <c r="N3"/>
+      <c r="O3" s="2"/>
       <c r="P3"/>
-      <c r="Q3" s="4"/>
-      <c r="R3"/>
+      <c r="Q3"/>
+      <c r="R3" s="4"/>
       <c r="S3"/>
       <c r="T3"/>
       <c r="U3"/>
       <c r="V3"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="23"/>
       <c r="P4" s="10"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="29"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="11"/>
+      <c r="O5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="11"/>
       <c r="P5" s="11"/>
-      <c r="Q5" s="30" t="s">
+      <c r="Q5" s="11"/>
+      <c r="R5" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="11"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="11"/>
+      <c r="O6" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="11"/>
       <c r="P6" s="11"/>
-      <c r="Q6" s="30" t="s">
+      <c r="Q6" s="11"/>
+      <c r="R6" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="11"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W6" s="11"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="27"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="11"/>
+      <c r="O7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="11"/>
       <c r="P7" s="11"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="30"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="11"/>
+      <c r="O8" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="11"/>
       <c r="P8" s="11"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="30"/>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="27"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-      <c r="N9" s="24" t="s">
+      <c r="N9" s="11"/>
+      <c r="O9" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="11"/>
       <c r="P9" s="11"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="30"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9" s="11"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="11"/>
-      <c r="Q10" s="30"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q10" s="11"/>
+      <c r="R10" s="30"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="26"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="23"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="29"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>51</v>
       </c>
@@ -1207,26 +1230,27 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="27"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="24"/>
       <c r="P12" s="11"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="12"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="30"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W12" s="12"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>52</v>
       </c>
@@ -1235,50 +1259,52 @@
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="27"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="24"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="12"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="31"/>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13" s="12"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="25"/>
       <c r="P14" s="13"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="32"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
-    </row>
-    <row r="15" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
@@ -1289,34 +1315,35 @@
       <c r="D15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="35"/>
       <c r="G15" s="35"/>
-      <c r="H15" s="36" t="s">
+      <c r="H15" s="35"/>
+      <c r="I15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="35"/>
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
       <c r="M15" s="35"/>
-      <c r="N15" s="34" t="s">
+      <c r="N15" s="35"/>
+      <c r="O15" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="O15" s="35"/>
       <c r="P15" s="35"/>
-      <c r="Q15" s="37" t="s">
+      <c r="Q15" s="35"/>
+      <c r="R15" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
-    </row>
-    <row r="16" spans="1:22" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="W15" s="11"/>
+    </row>
+    <row r="16" spans="1:23" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>23</v>
       </c>
@@ -1327,34 +1354,35 @@
       <c r="D16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="22"/>
+      <c r="F16" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
-      <c r="N16" s="34" t="s">
+      <c r="N16" s="22"/>
+      <c r="O16" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="O16" s="22"/>
       <c r="P16" s="22"/>
-      <c r="Q16" s="37" t="s">
+      <c r="Q16" s="22"/>
+      <c r="R16" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="11"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
-    </row>
-    <row r="17" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="11"/>
+    </row>
+    <row r="17" spans="1:23" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
@@ -1365,34 +1393,35 @@
       <c r="D17" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="22"/>
+      <c r="F17" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="22"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
-      <c r="N17" s="34" t="s">
+      <c r="N17" s="22"/>
+      <c r="O17" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="22"/>
       <c r="P17" s="22"/>
-      <c r="Q17" s="37" t="s">
+      <c r="Q17" s="22"/>
+      <c r="R17" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-    </row>
-    <row r="18" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="1:23" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>23</v>
       </c>
@@ -1403,34 +1432,35 @@
       <c r="D18" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="22"/>
+      <c r="I18" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="22"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="22"/>
+      <c r="O18" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="22"/>
       <c r="P18" s="22"/>
-      <c r="Q18" s="37" t="s">
+      <c r="Q18" s="22"/>
+      <c r="R18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="R18" s="11"/>
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
-    </row>
-    <row r="19" spans="1:22" s="16" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="1:23" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>23</v>
       </c>
@@ -1439,34 +1469,35 @@
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="I19" s="22"/>
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
-      <c r="N19" s="34" t="s">
+      <c r="N19" s="22"/>
+      <c r="O19" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="O19" s="22"/>
       <c r="P19" s="22"/>
-      <c r="Q19" s="34" t="s">
+      <c r="Q19" s="22"/>
+      <c r="R19" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
-    </row>
-    <row r="20" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>23</v>
       </c>
@@ -1475,48 +1506,50 @@
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="24"/>
       <c r="P20" s="11"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="30"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="26"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="23"/>
       <c r="P21" s="10"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="29"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>